<commit_message>
Planilha de Desfazimento e Org. de Baixas
- O sistema busca a ultima planilha que foi criada no banco.

- Ao clicar no botão de Continuar Edição, ele automaticamente passa a editar a planilha mais atual do sistema.

- Ao clicar em Organização de Baixas, ele faz os agrupamentos da planilha mais atual também.
</commit_message>
<xml_diff>
--- a/testes_planilhas/RELATÓRIO DE DESFAZIMENTO DE BENS MÓVEIS PATRIMONIAIS DE 2014.xlsx
+++ b/testes_planilhas/RELATÓRIO DE DESFAZIMENTO DE BENS MÓVEIS PATRIMONIAIS DE 2014.xlsx
@@ -443,7 +443,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -511,38 +511,354 @@
       </c>
     </row>
     <row r="3" ht="30" customHeight="1">
-      <c r="A3" s="3" t="n">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>Nº DE ORDEM</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>TOMBO</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="inlineStr">
+        <is>
+          <t>DESCRIÇÃO DO BEM</t>
+        </is>
+      </c>
+      <c r="D3" s="3" t="inlineStr">
+        <is>
+          <t>DATA DA AQUISIÇÃO</t>
+        </is>
+      </c>
+      <c r="E3" s="3" t="inlineStr">
+        <is>
+          <t>DOCUMENTO FISCAL</t>
+        </is>
+      </c>
+      <c r="F3" s="3" t="inlineStr">
+        <is>
+          <t>UNIDADE RESPONSÁVEL</t>
+        </is>
+      </c>
+      <c r="G3" s="3" t="inlineStr">
+        <is>
+          <t>CLASSIFICAÇÃO</t>
+        </is>
+      </c>
+      <c r="H3" s="3" t="inlineStr">
+        <is>
+          <t>DESTINAÇÃO</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="30" customHeight="1">
+      <c r="A4" s="3" t="inlineStr">
+        <is>
+          <t>Nº DE ORDEM</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>TOMBO</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="inlineStr">
+        <is>
+          <t>DESCRIÇÃO DO BEM</t>
+        </is>
+      </c>
+      <c r="D4" s="3" t="inlineStr">
+        <is>
+          <t>DATA DA AQUISIÇÃO</t>
+        </is>
+      </c>
+      <c r="E4" s="3" t="inlineStr">
+        <is>
+          <t>DOCUMENTO FISCAL</t>
+        </is>
+      </c>
+      <c r="F4" s="3" t="inlineStr">
+        <is>
+          <t>UNIDADE RESPONSÁVEL</t>
+        </is>
+      </c>
+      <c r="G4" s="3" t="inlineStr">
+        <is>
+          <t>CLASSIFICAÇÃO</t>
+        </is>
+      </c>
+      <c r="H4" s="3" t="inlineStr">
+        <is>
+          <t>DESTINAÇÃO</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="30" customHeight="1">
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>Nº DE ORDEM</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>TOMBO</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="inlineStr">
+        <is>
+          <t>DESCRIÇÃO DO BEM</t>
+        </is>
+      </c>
+      <c r="D5" s="3" t="inlineStr">
+        <is>
+          <t>DATA DA AQUISIÇÃO</t>
+        </is>
+      </c>
+      <c r="E5" s="3" t="inlineStr">
+        <is>
+          <t>DOCUMENTO FISCAL</t>
+        </is>
+      </c>
+      <c r="F5" s="3" t="inlineStr">
+        <is>
+          <t>UNIDADE RESPONSÁVEL</t>
+        </is>
+      </c>
+      <c r="G5" s="3" t="inlineStr">
+        <is>
+          <t>CLASSIFICAÇÃO</t>
+        </is>
+      </c>
+      <c r="H5" s="3" t="inlineStr">
+        <is>
+          <t>DESTINAÇÃO</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="30" customHeight="1">
+      <c r="A6" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="n">
+      <c r="B6" s="3" t="n">
         <v>100119</v>
       </c>
-      <c r="C3" s="3" t="inlineStr">
+      <c r="C6" s="3" t="inlineStr">
         <is>
           <t>Câmera DSLR Canon EOS Rebel T7+</t>
         </is>
       </c>
-      <c r="D3" s="3" t="inlineStr">
+      <c r="D6" s="3" t="inlineStr">
         <is>
           <t>30/11/2022</t>
         </is>
       </c>
-      <c r="E3" s="3" t="inlineStr">
+      <c r="E6" s="3" t="inlineStr">
         <is>
           <t>NF-e 51009</t>
         </is>
       </c>
-      <c r="F3" s="3" t="inlineStr">
+      <c r="F6" s="3" t="inlineStr">
         <is>
           <t>Pró-Reitoria de Assuntos Estudantis (PROAES)</t>
         </is>
       </c>
-      <c r="G3" s="3" t="inlineStr">
+      <c r="G6" s="3" t="inlineStr">
         <is>
           <t>Irrecuperável</t>
         </is>
       </c>
-      <c r="H3" s="3" t="inlineStr">
+      <c r="H6" s="3" t="inlineStr">
+        <is>
+          <t>Alienação/Leilão</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="30" customHeight="1">
+      <c r="A7" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B7" s="3" t="n">
+        <v>100103</v>
+      </c>
+      <c r="C7" s="3" t="inlineStr">
+        <is>
+          <t>Mesa de escritório 1.20m x 0.60m, cor carvalho</t>
+        </is>
+      </c>
+      <c r="D7" s="3" t="inlineStr">
+        <is>
+          <t>20/11/2021</t>
+        </is>
+      </c>
+      <c r="E7" s="3" t="inlineStr">
+        <is>
+          <t>NF-e 33210</t>
+        </is>
+      </c>
+      <c r="F7" s="3" t="inlineStr">
+        <is>
+          <t>Diretoria de Comunicação (DECOM)</t>
+        </is>
+      </c>
+      <c r="G7" s="3" t="inlineStr">
+        <is>
+          <t>Irrecuperável</t>
+        </is>
+      </c>
+      <c r="H7" s="3" t="inlineStr">
+        <is>
+          <t>Alienação/Leilão</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" ht="30" customHeight="1">
+      <c r="A8" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B8" s="3" t="n">
+        <v>199887</v>
+      </c>
+      <c r="C8" s="3" t="inlineStr">
+        <is>
+          <t>Maca hospitalar simples com rodízios</t>
+        </is>
+      </c>
+      <c r="D8" s="3" t="inlineStr">
+        <is>
+          <t>15/12/2021</t>
+        </is>
+      </c>
+      <c r="E8" s="3" t="inlineStr">
+        <is>
+          <t>NF-e 34567</t>
+        </is>
+      </c>
+      <c r="F8" s="3" t="inlineStr">
+        <is>
+          <t>Centro de Ciências da Saúde e do Desporto (CCSD)</t>
+        </is>
+      </c>
+      <c r="G8" s="3" t="inlineStr">
+        <is>
+          <t>Irrecuperável</t>
+        </is>
+      </c>
+      <c r="H8" s="3" t="inlineStr">
+        <is>
+          <t>Alienação/Leilão</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="30" customHeight="1">
+      <c r="A9" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="B9" s="3" t="n">
+        <v>134567</v>
+      </c>
+      <c r="C9" s="3" t="inlineStr">
+        <is>
+          <t>Arquivo de aço com 4 gavetas, para pasta suspensa</t>
+        </is>
+      </c>
+      <c r="D9" s="3" t="inlineStr">
+        <is>
+          <t>19/05/2017</t>
+        </is>
+      </c>
+      <c r="E9" s="3" t="inlineStr">
+        <is>
+          <t>NF-e 8123</t>
+        </is>
+      </c>
+      <c r="F9" s="3" t="inlineStr">
+        <is>
+          <t>Diretoria de Sistemas de Informação (DSI)</t>
+        </is>
+      </c>
+      <c r="G9" s="3" t="inlineStr">
+        <is>
+          <t>Irrecuperável</t>
+        </is>
+      </c>
+      <c r="H9" s="3" t="inlineStr">
+        <is>
+          <t>Alienação/Leilão</t>
+        </is>
+      </c>
+    </row>
+    <row r="10" ht="30" customHeight="1">
+      <c r="A10" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="B10" s="3" t="n">
+        <v>112233</v>
+      </c>
+      <c r="C10" s="3" t="inlineStr">
+        <is>
+          <t>Multímetro Digital Minipa ET-2042E</t>
+        </is>
+      </c>
+      <c r="D10" s="3" t="inlineStr">
+        <is>
+          <t>10/05/2023</t>
+        </is>
+      </c>
+      <c r="E10" s="3" t="inlineStr">
+        <is>
+          <t>NF-e 54001</t>
+        </is>
+      </c>
+      <c r="F10" s="3" t="inlineStr">
+        <is>
+          <t>Coordenação do Curso de Engenharia Elétrica</t>
+        </is>
+      </c>
+      <c r="G10" s="3" t="inlineStr">
+        <is>
+          <t>Irrecuperável</t>
+        </is>
+      </c>
+      <c r="H10" s="3" t="inlineStr">
+        <is>
+          <t>Alienação/Leilão</t>
+        </is>
+      </c>
+    </row>
+    <row r="11" ht="30" customHeight="1">
+      <c r="A11" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3" t="n">
+        <v>121212</v>
+      </c>
+      <c r="C11" s="3" t="inlineStr">
+        <is>
+          <t>Switch de rede 24 portas Gigabit, TP-Link</t>
+        </is>
+      </c>
+      <c r="D11" s="3" t="inlineStr">
+        <is>
+          <t>07/07/2022</t>
+        </is>
+      </c>
+      <c r="E11" s="3" t="inlineStr">
+        <is>
+          <t>NF-e 48500</t>
+        </is>
+      </c>
+      <c r="F11" s="3" t="inlineStr">
+        <is>
+          <t>Pró-Reitoria de Desenvolvimento e Gestão de Pessoas (PRODGEP)</t>
+        </is>
+      </c>
+      <c r="G11" s="3" t="inlineStr">
+        <is>
+          <t>Irrecuperável</t>
+        </is>
+      </c>
+      <c r="H11" s="3" t="inlineStr">
         <is>
           <t>Alienação/Leilão</t>
         </is>

</xml_diff>